<commit_message>
adicionamento de mais 2 tabelas ao arquivo
</commit_message>
<xml_diff>
--- a/Dicionario de dados/dicionario_dados_academia.xlsx
+++ b/Dicionario de dados/dicionario_dados_academia.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gffernandes\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel Casa\Desktop\Assinatura_academia_SATC-main\Dicionario de dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A5E0BF6-FAAA-4A3E-B208-E190300227C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B48DC75B-29B3-4ED3-809D-59B50E7A47E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8A75A3C3-1CC3-42DF-908E-18684CFF6B01}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{8A75A3C3-1CC3-42DF-908E-18684CFF6B01}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="118">
   <si>
     <t>Tabela</t>
   </si>
@@ -318,13 +318,85 @@
   </si>
   <si>
     <t>decimal(32,2)</t>
+  </si>
+  <si>
+    <t>enum</t>
+  </si>
+  <si>
+    <t>desc.tipo_p</t>
+  </si>
+  <si>
+    <t>Contratos</t>
+  </si>
+  <si>
+    <t>Tabela responsável por armazenar os dados dos contratos dos clientes</t>
+  </si>
+  <si>
+    <t>cd_contrato</t>
+  </si>
+  <si>
+    <t>Código do contrato</t>
+  </si>
+  <si>
+    <t>Código do funcionario</t>
+  </si>
+  <si>
+    <t>Código do cliente</t>
+  </si>
+  <si>
+    <t>Código do plano</t>
+  </si>
+  <si>
+    <t>Aulas</t>
+  </si>
+  <si>
+    <t>Tabela responsável por armazenar os dados das aulas</t>
+  </si>
+  <si>
+    <t>cd_aula</t>
+  </si>
+  <si>
+    <t>Código de identificador da aula</t>
+  </si>
+  <si>
+    <t>nm_aula</t>
+  </si>
+  <si>
+    <t>Nome da aula</t>
+  </si>
+  <si>
+    <t>dt_inicio</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> dt_fim</t>
+  </si>
+  <si>
+    <t>cd_instrutor</t>
+  </si>
+  <si>
+    <t>capacidade</t>
+  </si>
+  <si>
+    <t>Descrição da aula</t>
+  </si>
+  <si>
+    <t>Data e horario de inicio da aula</t>
+  </si>
+  <si>
+    <t>Data e horario de fim da aula</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>Codigo ddo funcionario(intruto do aluno)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -343,6 +415,12 @@
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.14999847407452621"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -421,6 +499,24 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -433,25 +529,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -459,9 +540,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -777,10 +855,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A588904-58D6-4340-A48F-92FCD18181A8}">
-  <dimension ref="A1:H142"/>
+  <dimension ref="A1:H143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="E93" sqref="E93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,74 +871,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="15" t="s">
+      <c r="B4" s="18"/>
+      <c r="C4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="G4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="H4" s="9" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="7"/>
+      <c r="B5" s="13"/>
       <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
@@ -879,14 +957,14 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="7"/>
+      <c r="B6" s="13"/>
       <c r="C6" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="5" t="s">
         <v>38</v>
       </c>
       <c r="E6" s="2"/>
@@ -897,14 +975,14 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="7"/>
+      <c r="B7" s="13"/>
       <c r="C7" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="10" t="s">
         <v>59</v>
       </c>
       <c r="E7" s="2" t="s">
@@ -917,14 +995,14 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="7"/>
+      <c r="B8" s="13"/>
       <c r="C8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="5" t="s">
         <v>38</v>
       </c>
       <c r="E8" s="2"/>
@@ -935,14 +1013,14 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="7"/>
+      <c r="B9" s="13"/>
       <c r="C9" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="5" t="s">
         <v>60</v>
       </c>
       <c r="E9" s="2"/>
@@ -953,14 +1031,14 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="7"/>
+      <c r="B10" s="13"/>
       <c r="C10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="9"/>
+      <c r="D10" s="5"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -969,14 +1047,14 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="7"/>
+      <c r="B11" s="13"/>
       <c r="C11" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="5" t="s">
         <v>49</v>
       </c>
       <c r="E11" s="2"/>
@@ -987,14 +1065,14 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="7"/>
+      <c r="B12" s="13"/>
       <c r="C12" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="9"/>
+      <c r="D12" s="5"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -1003,174 +1081,174 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="11" t="s">
+      <c r="B14" s="16"/>
+      <c r="C14" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F15" s="12" t="s">
+      <c r="B15" s="15"/>
+      <c r="C15" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" s="14"/>
-      <c r="F16" s="12" t="s">
+      <c r="B16" s="15"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="7"/>
+      <c r="F16" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F17" s="12" t="s">
+      <c r="B17" s="15"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="14"/>
-      <c r="F18" s="12" t="s">
+      <c r="B18" s="15"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="7"/>
+      <c r="F18" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="17"/>
-      <c r="C24" s="15" t="s">
+      <c r="B24" s="18"/>
+      <c r="C24" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="15" t="s">
+      <c r="D24" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E24" s="15" t="s">
+      <c r="E24" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F24" s="15" t="s">
+      <c r="F24" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G24" s="15" t="s">
+      <c r="G24" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H24" s="15" t="s">
+      <c r="H24" s="9" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="7"/>
+      <c r="B25" s="13"/>
       <c r="C25" s="2" t="s">
         <v>11</v>
       </c>
@@ -1189,10 +1267,10 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="B26" s="7"/>
+      <c r="B26" s="13"/>
       <c r="C26" s="2" t="s">
         <v>57</v>
       </c>
@@ -1209,14 +1287,14 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="7"/>
+      <c r="B27" s="13"/>
       <c r="C27" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D27" s="18" t="s">
+      <c r="D27" s="10" t="s">
         <v>59</v>
       </c>
       <c r="E27" s="2"/>
@@ -1227,14 +1305,14 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="7"/>
+      <c r="B28" s="13"/>
       <c r="C28" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D28" s="9" t="s">
+      <c r="D28" s="5" t="s">
         <v>38</v>
       </c>
       <c r="E28" s="2"/>
@@ -1245,14 +1323,14 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="7"/>
+      <c r="B29" s="13"/>
       <c r="C29" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D29" s="9" t="s">
+      <c r="D29" s="5" t="s">
         <v>60</v>
       </c>
       <c r="E29" s="2"/>
@@ -1263,10 +1341,10 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="B30" s="7"/>
+      <c r="B30" s="13"/>
       <c r="C30" s="2" t="s">
         <v>11</v>
       </c>
@@ -1279,10 +1357,10 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="B31" s="7"/>
+      <c r="B31" s="13"/>
       <c r="C31" s="2" t="s">
         <v>69</v>
       </c>
@@ -1297,10 +1375,10 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="B32" s="7"/>
+      <c r="B32" s="13"/>
       <c r="C32" s="2" t="s">
         <v>42</v>
       </c>
@@ -1313,10 +1391,10 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="B33" s="7"/>
+      <c r="B33" s="13"/>
       <c r="C33" s="2" t="s">
         <v>42</v>
       </c>
@@ -1331,10 +1409,10 @@
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="B34" s="7"/>
+      <c r="B34" s="13"/>
       <c r="C34" s="2" t="s">
         <v>42</v>
       </c>
@@ -1349,10 +1427,10 @@
       </c>
     </row>
     <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
+      <c r="A35" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="B35" s="7"/>
+      <c r="B35" s="13"/>
       <c r="C35" s="2" t="s">
         <v>42</v>
       </c>
@@ -1367,150 +1445,150 @@
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="10" t="s">
+      <c r="A36" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B36" s="10"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
-      <c r="H36" s="10"/>
+      <c r="B36" s="16"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="16"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="10" t="s">
+      <c r="A37" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B37" s="10"/>
-      <c r="C37" s="11" t="s">
+      <c r="B37" s="16"/>
+      <c r="C37" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D37" s="11" t="s">
+      <c r="D37" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E37" s="11" t="s">
+      <c r="E37" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F37" s="10" t="s">
+      <c r="F37" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G37" s="10"/>
-      <c r="H37" s="10"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="16"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="12" t="s">
+      <c r="A38" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B38" s="12"/>
-      <c r="C38" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F38" s="12" t="s">
+      <c r="B38" s="15"/>
+      <c r="C38" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G38" s="12"/>
-      <c r="H38" s="12"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="15"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="12" t="s">
+      <c r="A39" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B39" s="12"/>
-      <c r="C39" s="13"/>
-      <c r="D39" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="E39" s="14"/>
-      <c r="F39" s="12" t="s">
+      <c r="B39" s="15"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E39" s="7"/>
+      <c r="F39" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G39" s="12"/>
-      <c r="H39" s="12"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="15"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="12" t="s">
+      <c r="A40" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B40" s="12"/>
-      <c r="C40" s="13"/>
-      <c r="D40" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="E40" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F40" s="12" t="s">
+      <c r="B40" s="15"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F40" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G40" s="12"/>
-      <c r="H40" s="12"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="15"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="12" t="s">
+      <c r="A41" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B41" s="12"/>
-      <c r="C41" s="13"/>
-      <c r="D41" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="E41" s="14"/>
-      <c r="F41" s="12" t="s">
+      <c r="B41" s="15"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E41" s="7"/>
+      <c r="F41" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G41" s="12"/>
-      <c r="H41" s="12"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="15"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="B43" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="7"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="13"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B44" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="C44" s="7"/>
-      <c r="D44" s="7"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="7"/>
-      <c r="G44" s="7"/>
-      <c r="H44" s="7"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="13"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="8" t="s">
+      <c r="A45" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B45" s="8"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="8"/>
-      <c r="F45" s="8"/>
-      <c r="G45" s="8"/>
-      <c r="H45" s="8"/>
+      <c r="B45" s="14"/>
+      <c r="C45" s="14"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="14"/>
+      <c r="G45" s="14"/>
+      <c r="H45" s="14"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="6" t="s">
+      <c r="A46" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B46" s="6"/>
+      <c r="B46" s="12"/>
       <c r="C46" s="1" t="s">
         <v>6</v>
       </c>
@@ -1531,10 +1609,10 @@
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="7" t="s">
+      <c r="A47" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="B47" s="7"/>
+      <c r="B47" s="13"/>
       <c r="C47" s="2" t="s">
         <v>11</v>
       </c>
@@ -1553,10 +1631,10 @@
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="7" t="s">
+      <c r="A48" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="B48" s="7"/>
+      <c r="B48" s="13"/>
       <c r="C48" s="2" t="s">
         <v>57</v>
       </c>
@@ -1571,10 +1649,10 @@
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="7" t="s">
+      <c r="A49" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="B49" s="7"/>
+      <c r="B49" s="13"/>
       <c r="C49" s="2" t="s">
         <v>92</v>
       </c>
@@ -1589,14 +1667,14 @@
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="7" t="s">
+      <c r="A50" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="B50" s="7"/>
+      <c r="B50" s="13"/>
       <c r="C50" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D50" s="9">
+      <c r="D50" s="5">
         <v>32.200000000000003</v>
       </c>
       <c r="E50" s="2"/>
@@ -1607,14 +1685,16 @@
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="7" t="s">
+      <c r="A51" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="B51" s="7"/>
+      <c r="B51" s="13"/>
       <c r="C51" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D51" s="2"/>
+        <v>94</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
@@ -1623,150 +1703,150 @@
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="6" t="s">
+      <c r="A52" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B52" s="6"/>
-      <c r="C52" s="6"/>
-      <c r="D52" s="6"/>
-      <c r="E52" s="6"/>
-      <c r="F52" s="6"/>
-      <c r="G52" s="6"/>
-      <c r="H52" s="6"/>
+      <c r="B52" s="16"/>
+      <c r="C52" s="16"/>
+      <c r="D52" s="16"/>
+      <c r="E52" s="16"/>
+      <c r="F52" s="16"/>
+      <c r="G52" s="16"/>
+      <c r="H52" s="16"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="6" t="s">
+      <c r="A53" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B53" s="6"/>
-      <c r="C53" s="1" t="s">
+      <c r="B53" s="16"/>
+      <c r="C53" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="D53" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E53" s="1" t="s">
+      <c r="E53" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F53" s="6" t="s">
+      <c r="F53" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G53" s="6"/>
-      <c r="H53" s="6"/>
+      <c r="G53" s="16"/>
+      <c r="H53" s="16"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="5" t="s">
+      <c r="A54" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B54" s="5"/>
-      <c r="C54" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D54" s="3"/>
-      <c r="E54" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F54" s="5" t="s">
+      <c r="B54" s="15"/>
+      <c r="C54" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D54" s="7"/>
+      <c r="E54" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F54" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G54" s="5"/>
-      <c r="H54" s="5"/>
+      <c r="G54" s="15"/>
+      <c r="H54" s="15"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="5" t="s">
+      <c r="A55" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B55" s="5"/>
-      <c r="C55" s="4"/>
-      <c r="D55" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E55" s="3"/>
-      <c r="F55" s="5" t="s">
+      <c r="B55" s="15"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E55" s="7"/>
+      <c r="F55" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G55" s="5"/>
-      <c r="H55" s="5"/>
+      <c r="G55" s="15"/>
+      <c r="H55" s="15"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="5" t="s">
+      <c r="A56" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B56" s="5"/>
-      <c r="C56" s="4"/>
-      <c r="D56" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F56" s="5" t="s">
+      <c r="B56" s="15"/>
+      <c r="C56" s="8"/>
+      <c r="D56" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E56" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F56" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G56" s="5"/>
-      <c r="H56" s="5"/>
+      <c r="G56" s="15"/>
+      <c r="H56" s="15"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="5" t="s">
+      <c r="A57" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B57" s="5"/>
-      <c r="C57" s="4"/>
-      <c r="D57" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E57" s="3"/>
-      <c r="F57" s="5" t="s">
+      <c r="B57" s="15"/>
+      <c r="C57" s="8"/>
+      <c r="D57" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E57" s="7"/>
+      <c r="F57" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G57" s="5"/>
-      <c r="H57" s="5"/>
+      <c r="G57" s="15"/>
+      <c r="H57" s="15"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B59" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C59" s="7"/>
-      <c r="D59" s="7"/>
-      <c r="E59" s="7"/>
-      <c r="F59" s="7"/>
-      <c r="G59" s="7"/>
-      <c r="H59" s="7"/>
+      <c r="B59" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C59" s="13"/>
+      <c r="D59" s="13"/>
+      <c r="E59" s="13"/>
+      <c r="F59" s="13"/>
+      <c r="G59" s="13"/>
+      <c r="H59" s="13"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B60" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C60" s="7"/>
-      <c r="D60" s="7"/>
-      <c r="E60" s="7"/>
-      <c r="F60" s="7"/>
-      <c r="G60" s="7"/>
-      <c r="H60" s="7"/>
+      <c r="B60" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C60" s="13"/>
+      <c r="D60" s="13"/>
+      <c r="E60" s="13"/>
+      <c r="F60" s="13"/>
+      <c r="G60" s="13"/>
+      <c r="H60" s="13"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="8" t="s">
+      <c r="A61" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B61" s="8"/>
-      <c r="C61" s="8"/>
-      <c r="D61" s="8"/>
-      <c r="E61" s="8"/>
-      <c r="F61" s="8"/>
-      <c r="G61" s="8"/>
-      <c r="H61" s="8"/>
+      <c r="B61" s="14"/>
+      <c r="C61" s="14"/>
+      <c r="D61" s="14"/>
+      <c r="E61" s="14"/>
+      <c r="F61" s="14"/>
+      <c r="G61" s="14"/>
+      <c r="H61" s="14"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="6" t="s">
+      <c r="A62" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B62" s="6"/>
+      <c r="B62" s="12"/>
       <c r="C62" s="1" t="s">
         <v>6</v>
       </c>
@@ -1787,10 +1867,10 @@
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B63" s="7"/>
+      <c r="A63" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B63" s="13"/>
       <c r="C63" s="2" t="s">
         <v>11</v>
       </c>
@@ -1805,52 +1885,72 @@
       </c>
       <c r="G63" s="2"/>
       <c r="H63" s="2" t="s">
-        <v>14</v>
+        <v>99</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B64" s="7"/>
+      <c r="A64" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B64" s="13"/>
       <c r="C64" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>12</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="E64" s="2"/>
       <c r="F64" s="2"/>
-      <c r="G64" s="2"/>
+      <c r="G64" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="H64" s="2" t="s">
-        <v>18</v>
+        <v>100</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="7"/>
-      <c r="B65" s="7"/>
-      <c r="C65" s="2"/>
-      <c r="D65" s="2"/>
+      <c r="A65" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B65" s="13"/>
+      <c r="C65" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
-      <c r="G65" s="2"/>
-      <c r="H65" s="2"/>
+      <c r="G65" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H65" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" s="7"/>
-      <c r="B66" s="7"/>
-      <c r="C66" s="2"/>
-      <c r="D66" s="2"/>
+      <c r="A66" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B66" s="13"/>
+      <c r="C66" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
-      <c r="G66" s="2"/>
-      <c r="H66" s="2"/>
+      <c r="G66" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H66" s="2" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" s="7"/>
-      <c r="B67" s="7"/>
+      <c r="A67" s="13"/>
+      <c r="B67" s="13"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
@@ -1859,8 +1959,8 @@
       <c r="H67" s="2"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" s="7"/>
-      <c r="B68" s="7"/>
+      <c r="A68" s="13"/>
+      <c r="B68" s="13"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
@@ -1869,150 +1969,150 @@
       <c r="H68" s="2"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" s="6" t="s">
+      <c r="A69" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B69" s="6"/>
-      <c r="C69" s="6"/>
-      <c r="D69" s="6"/>
-      <c r="E69" s="6"/>
-      <c r="F69" s="6"/>
-      <c r="G69" s="6"/>
-      <c r="H69" s="6"/>
+      <c r="B69" s="16"/>
+      <c r="C69" s="16"/>
+      <c r="D69" s="16"/>
+      <c r="E69" s="16"/>
+      <c r="F69" s="16"/>
+      <c r="G69" s="16"/>
+      <c r="H69" s="16"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="6" t="s">
+      <c r="A70" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B70" s="6"/>
-      <c r="C70" s="1" t="s">
+      <c r="B70" s="16"/>
+      <c r="C70" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D70" s="1" t="s">
+      <c r="D70" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E70" s="1" t="s">
+      <c r="E70" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F70" s="6" t="s">
+      <c r="F70" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G70" s="6"/>
-      <c r="H70" s="6"/>
+      <c r="G70" s="16"/>
+      <c r="H70" s="16"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="5" t="s">
+      <c r="A71" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B71" s="5"/>
-      <c r="C71" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D71" s="3"/>
-      <c r="E71" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F71" s="5" t="s">
+      <c r="B71" s="15"/>
+      <c r="C71" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D71" s="7"/>
+      <c r="E71" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F71" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G71" s="5"/>
-      <c r="H71" s="5"/>
+      <c r="G71" s="15"/>
+      <c r="H71" s="15"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" s="5" t="s">
+      <c r="A72" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B72" s="5"/>
-      <c r="C72" s="4"/>
-      <c r="D72" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E72" s="3"/>
-      <c r="F72" s="5" t="s">
+      <c r="B72" s="15"/>
+      <c r="C72" s="8"/>
+      <c r="D72" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E72" s="7"/>
+      <c r="F72" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G72" s="5"/>
-      <c r="H72" s="5"/>
+      <c r="G72" s="15"/>
+      <c r="H72" s="15"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="5" t="s">
+      <c r="A73" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B73" s="5"/>
-      <c r="C73" s="4"/>
-      <c r="D73" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E73" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F73" s="5" t="s">
+      <c r="B73" s="15"/>
+      <c r="C73" s="8"/>
+      <c r="D73" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E73" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F73" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G73" s="5"/>
-      <c r="H73" s="5"/>
+      <c r="G73" s="15"/>
+      <c r="H73" s="15"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="5" t="s">
+      <c r="A74" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B74" s="5"/>
-      <c r="C74" s="4"/>
-      <c r="D74" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E74" s="3"/>
-      <c r="F74" s="5" t="s">
+      <c r="B74" s="15"/>
+      <c r="C74" s="8"/>
+      <c r="D74" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E74" s="7"/>
+      <c r="F74" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G74" s="5"/>
-      <c r="H74" s="5"/>
+      <c r="G74" s="15"/>
+      <c r="H74" s="15"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B76" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C76" s="7"/>
-      <c r="D76" s="7"/>
-      <c r="E76" s="7"/>
-      <c r="F76" s="7"/>
-      <c r="G76" s="7"/>
-      <c r="H76" s="7"/>
+      <c r="B76" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C76" s="13"/>
+      <c r="D76" s="13"/>
+      <c r="E76" s="13"/>
+      <c r="F76" s="13"/>
+      <c r="G76" s="13"/>
+      <c r="H76" s="13"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B77" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C77" s="7"/>
-      <c r="D77" s="7"/>
-      <c r="E77" s="7"/>
-      <c r="F77" s="7"/>
-      <c r="G77" s="7"/>
-      <c r="H77" s="7"/>
+      <c r="B77" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="C77" s="13"/>
+      <c r="D77" s="13"/>
+      <c r="E77" s="13"/>
+      <c r="F77" s="13"/>
+      <c r="G77" s="13"/>
+      <c r="H77" s="13"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A78" s="8" t="s">
+      <c r="A78" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B78" s="8"/>
-      <c r="C78" s="8"/>
-      <c r="D78" s="8"/>
-      <c r="E78" s="8"/>
-      <c r="F78" s="8"/>
-      <c r="G78" s="8"/>
-      <c r="H78" s="8"/>
+      <c r="B78" s="14"/>
+      <c r="C78" s="14"/>
+      <c r="D78" s="14"/>
+      <c r="E78" s="14"/>
+      <c r="F78" s="14"/>
+      <c r="G78" s="14"/>
+      <c r="H78" s="14"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A79" s="6" t="s">
+      <c r="A79" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B79" s="6"/>
+      <c r="B79" s="12"/>
       <c r="C79" s="1" t="s">
         <v>6</v>
       </c>
@@ -2033,10 +2133,10 @@
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A80" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B80" s="7"/>
+      <c r="A80" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="B80" s="13"/>
       <c r="C80" s="2" t="s">
         <v>11</v>
       </c>
@@ -2051,288 +2151,322 @@
       </c>
       <c r="G80" s="2"/>
       <c r="H80" s="2" t="s">
-        <v>14</v>
+        <v>106</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A81" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B81" s="7"/>
+      <c r="A81" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="B81" s="13"/>
       <c r="C81" s="2" t="s">
-        <v>16</v>
+        <v>57</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E81" s="2" t="s">
-        <v>12</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="E81" s="2"/>
       <c r="F81" s="2"/>
       <c r="G81" s="2"/>
       <c r="H81" s="2" t="s">
-        <v>18</v>
+        <v>108</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A82" s="7"/>
-      <c r="B82" s="7"/>
-      <c r="C82" s="2"/>
-      <c r="D82" s="2"/>
+      <c r="A82" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="B82" s="13"/>
+      <c r="C82" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="E82" s="2"/>
       <c r="F82" s="2"/>
       <c r="G82" s="2"/>
-      <c r="H82" s="2"/>
+      <c r="H82" s="2" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A83" s="7"/>
-      <c r="B83" s="7"/>
-      <c r="C83" s="2"/>
+      <c r="A83" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B83" s="13"/>
+      <c r="C83" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="D83" s="2"/>
       <c r="E83" s="2"/>
       <c r="F83" s="2"/>
       <c r="G83" s="2"/>
-      <c r="H83" s="2"/>
+      <c r="H83" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A84" s="7"/>
-      <c r="B84" s="7"/>
-      <c r="C84" s="2"/>
+      <c r="A84" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="B84" s="13"/>
+      <c r="C84" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="D84" s="2"/>
       <c r="E84" s="2"/>
       <c r="F84" s="2"/>
       <c r="G84" s="2"/>
-      <c r="H84" s="2"/>
+      <c r="H84" s="2" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A85" s="7"/>
-      <c r="B85" s="7"/>
-      <c r="C85" s="2"/>
+      <c r="A85" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="B85" s="13"/>
+      <c r="C85" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="D85" s="2"/>
-      <c r="E85" s="2"/>
+      <c r="E85" s="2" t="s">
+        <v>116</v>
+      </c>
       <c r="F85" s="2"/>
       <c r="G85" s="2"/>
-      <c r="H85" s="2"/>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A86" s="6" t="s">
+      <c r="H85" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="B86" s="13"/>
+      <c r="C86" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D86" s="2"/>
+      <c r="E86" s="2"/>
+      <c r="F86" s="2"/>
+      <c r="G86" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H86" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B86" s="6"/>
-      <c r="C86" s="6"/>
-      <c r="D86" s="6"/>
-      <c r="E86" s="6"/>
-      <c r="F86" s="6"/>
-      <c r="G86" s="6"/>
-      <c r="H86" s="6"/>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" s="6" t="s">
+      <c r="B87" s="16"/>
+      <c r="C87" s="16"/>
+      <c r="D87" s="16"/>
+      <c r="E87" s="16"/>
+      <c r="F87" s="16"/>
+      <c r="G87" s="16"/>
+      <c r="H87" s="16"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B87" s="6"/>
-      <c r="C87" s="1" t="s">
+      <c r="B88" s="16"/>
+      <c r="C88" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D87" s="1" t="s">
+      <c r="D88" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E87" s="1" t="s">
+      <c r="E88" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F87" s="6" t="s">
+      <c r="F88" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G87" s="6"/>
-      <c r="H87" s="6"/>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A88" s="5" t="s">
+      <c r="G88" s="16"/>
+      <c r="H88" s="16"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B88" s="5"/>
-      <c r="C88" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D88" s="3"/>
-      <c r="E88" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F88" s="5" t="s">
+      <c r="B89" s="15"/>
+      <c r="C89" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D89" s="7"/>
+      <c r="E89" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F89" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G88" s="5"/>
-      <c r="H88" s="5"/>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A89" s="5" t="s">
+      <c r="G89" s="15"/>
+      <c r="H89" s="15"/>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B89" s="5"/>
-      <c r="C89" s="4"/>
-      <c r="D89" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E89" s="3"/>
-      <c r="F89" s="5" t="s">
+      <c r="B90" s="15"/>
+      <c r="C90" s="8"/>
+      <c r="D90" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E90" s="7"/>
+      <c r="F90" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G89" s="5"/>
-      <c r="H89" s="5"/>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A90" s="5" t="s">
+      <c r="G90" s="15"/>
+      <c r="H90" s="15"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B90" s="5"/>
-      <c r="C90" s="4"/>
-      <c r="D90" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E90" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F90" s="5" t="s">
+      <c r="B91" s="15"/>
+      <c r="C91" s="8"/>
+      <c r="D91" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E91" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F91" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G90" s="5"/>
-      <c r="H90" s="5"/>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A91" s="5" t="s">
+      <c r="G91" s="15"/>
+      <c r="H91" s="15"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B91" s="5"/>
-      <c r="C91" s="4"/>
-      <c r="D91" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E91" s="3"/>
-      <c r="F91" s="5" t="s">
+      <c r="B92" s="15"/>
+      <c r="C92" s="8"/>
+      <c r="D92" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E92" s="7"/>
+      <c r="F92" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G91" s="5"/>
-      <c r="H91" s="5"/>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B93" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C93" s="7"/>
-      <c r="D93" s="7"/>
-      <c r="E93" s="7"/>
-      <c r="F93" s="7"/>
-      <c r="G93" s="7"/>
-      <c r="H93" s="7"/>
+      <c r="G92" s="15"/>
+      <c r="H92" s="15"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B94" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C94" s="13"/>
+      <c r="D94" s="13"/>
+      <c r="E94" s="13"/>
+      <c r="F94" s="13"/>
+      <c r="G94" s="13"/>
+      <c r="H94" s="13"/>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B94" s="7" t="s">
+      <c r="B95" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C94" s="7"/>
-      <c r="D94" s="7"/>
-      <c r="E94" s="7"/>
-      <c r="F94" s="7"/>
-      <c r="G94" s="7"/>
-      <c r="H94" s="7"/>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A95" s="8" t="s">
+      <c r="C95" s="13"/>
+      <c r="D95" s="13"/>
+      <c r="E95" s="13"/>
+      <c r="F95" s="13"/>
+      <c r="G95" s="13"/>
+      <c r="H95" s="13"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B95" s="8"/>
-      <c r="C95" s="8"/>
-      <c r="D95" s="8"/>
-      <c r="E95" s="8"/>
-      <c r="F95" s="8"/>
-      <c r="G95" s="8"/>
-      <c r="H95" s="8"/>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A96" s="6" t="s">
+      <c r="B96" s="14"/>
+      <c r="C96" s="14"/>
+      <c r="D96" s="14"/>
+      <c r="E96" s="14"/>
+      <c r="F96" s="14"/>
+      <c r="G96" s="14"/>
+      <c r="H96" s="14"/>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A97" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B96" s="6"/>
-      <c r="C96" s="1" t="s">
+      <c r="B97" s="12"/>
+      <c r="C97" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D96" s="1" t="s">
+      <c r="D97" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E96" s="1" t="s">
+      <c r="E97" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F96" s="1" t="s">
+      <c r="F97" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G96" s="1" t="s">
+      <c r="G97" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H96" s="1" t="s">
+      <c r="H97" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A97" s="7" t="s">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A98" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B97" s="7"/>
-      <c r="C97" s="2" t="s">
+      <c r="B98" s="13"/>
+      <c r="C98" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D97" s="2" t="s">
+      <c r="D98" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="E97" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F97" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G97" s="2"/>
-      <c r="H97" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A98" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B98" s="7"/>
-      <c r="C98" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D98" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="E98" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F98" s="2"/>
+      <c r="F98" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="G98" s="2"/>
       <c r="H98" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A99" s="7"/>
-      <c r="B99" s="7"/>
-      <c r="C99" s="2"/>
-      <c r="D99" s="2"/>
-      <c r="E99" s="2"/>
+      <c r="A99" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B99" s="13"/>
+      <c r="C99" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="F99" s="2"/>
       <c r="G99" s="2"/>
-      <c r="H99" s="2"/>
+      <c r="H99" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A100" s="7"/>
-      <c r="B100" s="7"/>
+      <c r="A100" s="13"/>
+      <c r="B100" s="13"/>
       <c r="C100" s="2"/>
       <c r="D100" s="2"/>
       <c r="E100" s="2"/>
@@ -2341,8 +2475,8 @@
       <c r="H100" s="2"/>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A101" s="7"/>
-      <c r="B101" s="7"/>
+      <c r="A101" s="13"/>
+      <c r="B101" s="13"/>
       <c r="C101" s="2"/>
       <c r="D101" s="2"/>
       <c r="E101" s="2"/>
@@ -2351,8 +2485,8 @@
       <c r="H101" s="2"/>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A102" s="7"/>
-      <c r="B102" s="7"/>
+      <c r="A102" s="13"/>
+      <c r="B102" s="13"/>
       <c r="C102" s="2"/>
       <c r="D102" s="2"/>
       <c r="E102" s="2"/>
@@ -2361,224 +2495,224 @@
       <c r="H102" s="2"/>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A103" s="6" t="s">
+      <c r="A103" s="13"/>
+      <c r="B103" s="13"/>
+      <c r="C103" s="2"/>
+      <c r="D103" s="2"/>
+      <c r="E103" s="2"/>
+      <c r="F103" s="2"/>
+      <c r="G103" s="2"/>
+      <c r="H103" s="2"/>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A104" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B103" s="6"/>
-      <c r="C103" s="6"/>
-      <c r="D103" s="6"/>
-      <c r="E103" s="6"/>
-      <c r="F103" s="6"/>
-      <c r="G103" s="6"/>
-      <c r="H103" s="6"/>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A104" s="6" t="s">
+      <c r="B104" s="12"/>
+      <c r="C104" s="12"/>
+      <c r="D104" s="12"/>
+      <c r="E104" s="12"/>
+      <c r="F104" s="12"/>
+      <c r="G104" s="12"/>
+      <c r="H104" s="12"/>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A105" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B104" s="6"/>
-      <c r="C104" s="1" t="s">
+      <c r="B105" s="12"/>
+      <c r="C105" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D104" s="1" t="s">
+      <c r="D105" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E104" s="1" t="s">
+      <c r="E105" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F104" s="6" t="s">
+      <c r="F105" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="G104" s="6"/>
-      <c r="H104" s="6"/>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A105" s="5" t="s">
+      <c r="G105" s="12"/>
+      <c r="H105" s="12"/>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A106" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B105" s="5"/>
-      <c r="C105" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D105" s="3"/>
-      <c r="E105" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F105" s="5" t="s">
+      <c r="B106" s="11"/>
+      <c r="C106" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D106" s="3"/>
+      <c r="E106" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F106" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="G105" s="5"/>
-      <c r="H105" s="5"/>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A106" s="5" t="s">
+      <c r="G106" s="11"/>
+      <c r="H106" s="11"/>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A107" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B106" s="5"/>
-      <c r="C106" s="4"/>
-      <c r="D106" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E106" s="3"/>
-      <c r="F106" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G106" s="5"/>
-      <c r="H106" s="5"/>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A107" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B107" s="5"/>
+      <c r="B107" s="11"/>
       <c r="C107" s="4"/>
       <c r="D107" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E107" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F107" s="5" t="s">
+      <c r="E107" s="3"/>
+      <c r="F107" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="G107" s="5"/>
-      <c r="H107" s="5"/>
+      <c r="G107" s="11"/>
+      <c r="H107" s="11"/>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A108" s="5" t="s">
+      <c r="A108" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B108" s="5"/>
+      <c r="B108" s="11"/>
       <c r="C108" s="4"/>
       <c r="D108" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E108" s="3"/>
-      <c r="F108" s="5" t="s">
+      <c r="E108" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F108" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="G108" s="5"/>
-      <c r="H108" s="5"/>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B110" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C110" s="7"/>
-      <c r="D110" s="7"/>
-      <c r="E110" s="7"/>
-      <c r="F110" s="7"/>
-      <c r="G110" s="7"/>
-      <c r="H110" s="7"/>
+      <c r="G108" s="11"/>
+      <c r="H108" s="11"/>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A109" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B109" s="11"/>
+      <c r="C109" s="4"/>
+      <c r="D109" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E109" s="3"/>
+      <c r="F109" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G109" s="11"/>
+      <c r="H109" s="11"/>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B111" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C111" s="13"/>
+      <c r="D111" s="13"/>
+      <c r="E111" s="13"/>
+      <c r="F111" s="13"/>
+      <c r="G111" s="13"/>
+      <c r="H111" s="13"/>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B111" s="7" t="s">
+      <c r="B112" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C111" s="7"/>
-      <c r="D111" s="7"/>
-      <c r="E111" s="7"/>
-      <c r="F111" s="7"/>
-      <c r="G111" s="7"/>
-      <c r="H111" s="7"/>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A112" s="8" t="s">
+      <c r="C112" s="13"/>
+      <c r="D112" s="13"/>
+      <c r="E112" s="13"/>
+      <c r="F112" s="13"/>
+      <c r="G112" s="13"/>
+      <c r="H112" s="13"/>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A113" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B112" s="8"/>
-      <c r="C112" s="8"/>
-      <c r="D112" s="8"/>
-      <c r="E112" s="8"/>
-      <c r="F112" s="8"/>
-      <c r="G112" s="8"/>
-      <c r="H112" s="8"/>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A113" s="6" t="s">
+      <c r="B113" s="14"/>
+      <c r="C113" s="14"/>
+      <c r="D113" s="14"/>
+      <c r="E113" s="14"/>
+      <c r="F113" s="14"/>
+      <c r="G113" s="14"/>
+      <c r="H113" s="14"/>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A114" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B113" s="6"/>
-      <c r="C113" s="1" t="s">
+      <c r="B114" s="12"/>
+      <c r="C114" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D113" s="1" t="s">
+      <c r="D114" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E113" s="1" t="s">
+      <c r="E114" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F113" s="1" t="s">
+      <c r="F114" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G113" s="1" t="s">
+      <c r="G114" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H113" s="1" t="s">
+      <c r="H114" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A114" s="7" t="s">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A115" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B114" s="7"/>
-      <c r="C114" s="2" t="s">
+      <c r="B115" s="13"/>
+      <c r="C115" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D114" s="2" t="s">
+      <c r="D115" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="E114" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F114" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G114" s="2"/>
-      <c r="H114" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A115" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B115" s="7"/>
-      <c r="C115" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D115" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="E115" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F115" s="2"/>
+      <c r="F115" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="G115" s="2"/>
       <c r="H115" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A116" s="7"/>
-      <c r="B116" s="7"/>
-      <c r="C116" s="2"/>
-      <c r="D116" s="2"/>
-      <c r="E116" s="2"/>
+      <c r="A116" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B116" s="13"/>
+      <c r="C116" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E116" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="F116" s="2"/>
       <c r="G116" s="2"/>
-      <c r="H116" s="2"/>
+      <c r="H116" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A117" s="7"/>
-      <c r="B117" s="7"/>
+      <c r="A117" s="13"/>
+      <c r="B117" s="13"/>
       <c r="C117" s="2"/>
       <c r="D117" s="2"/>
       <c r="E117" s="2"/>
@@ -2587,8 +2721,8 @@
       <c r="H117" s="2"/>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A118" s="7"/>
-      <c r="B118" s="7"/>
+      <c r="A118" s="13"/>
+      <c r="B118" s="13"/>
       <c r="C118" s="2"/>
       <c r="D118" s="2"/>
       <c r="E118" s="2"/>
@@ -2597,8 +2731,8 @@
       <c r="H118" s="2"/>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A119" s="7"/>
-      <c r="B119" s="7"/>
+      <c r="A119" s="13"/>
+      <c r="B119" s="13"/>
       <c r="C119" s="2"/>
       <c r="D119" s="2"/>
       <c r="E119" s="2"/>
@@ -2607,224 +2741,224 @@
       <c r="H119" s="2"/>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A120" s="6" t="s">
+      <c r="A120" s="13"/>
+      <c r="B120" s="13"/>
+      <c r="C120" s="2"/>
+      <c r="D120" s="2"/>
+      <c r="E120" s="2"/>
+      <c r="F120" s="2"/>
+      <c r="G120" s="2"/>
+      <c r="H120" s="2"/>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A121" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B120" s="6"/>
-      <c r="C120" s="6"/>
-      <c r="D120" s="6"/>
-      <c r="E120" s="6"/>
-      <c r="F120" s="6"/>
-      <c r="G120" s="6"/>
-      <c r="H120" s="6"/>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A121" s="6" t="s">
+      <c r="B121" s="12"/>
+      <c r="C121" s="12"/>
+      <c r="D121" s="12"/>
+      <c r="E121" s="12"/>
+      <c r="F121" s="12"/>
+      <c r="G121" s="12"/>
+      <c r="H121" s="12"/>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A122" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B121" s="6"/>
-      <c r="C121" s="1" t="s">
+      <c r="B122" s="12"/>
+      <c r="C122" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D121" s="1" t="s">
+      <c r="D122" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E121" s="1" t="s">
+      <c r="E122" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F121" s="6" t="s">
+      <c r="F122" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="G121" s="6"/>
-      <c r="H121" s="6"/>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A122" s="5" t="s">
+      <c r="G122" s="12"/>
+      <c r="H122" s="12"/>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A123" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B122" s="5"/>
-      <c r="C122" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D122" s="3"/>
-      <c r="E122" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F122" s="5" t="s">
+      <c r="B123" s="11"/>
+      <c r="C123" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D123" s="3"/>
+      <c r="E123" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F123" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="G122" s="5"/>
-      <c r="H122" s="5"/>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A123" s="5" t="s">
+      <c r="G123" s="11"/>
+      <c r="H123" s="11"/>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A124" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B123" s="5"/>
-      <c r="C123" s="4"/>
-      <c r="D123" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E123" s="3"/>
-      <c r="F123" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G123" s="5"/>
-      <c r="H123" s="5"/>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A124" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B124" s="5"/>
+      <c r="B124" s="11"/>
       <c r="C124" s="4"/>
       <c r="D124" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E124" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F124" s="5" t="s">
+      <c r="E124" s="3"/>
+      <c r="F124" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="G124" s="5"/>
-      <c r="H124" s="5"/>
+      <c r="G124" s="11"/>
+      <c r="H124" s="11"/>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A125" s="5" t="s">
+      <c r="A125" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B125" s="5"/>
+      <c r="B125" s="11"/>
       <c r="C125" s="4"/>
       <c r="D125" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E125" s="3"/>
-      <c r="F125" s="5" t="s">
+      <c r="E125" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F125" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="G125" s="5"/>
-      <c r="H125" s="5"/>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A127" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B127" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C127" s="7"/>
-      <c r="D127" s="7"/>
-      <c r="E127" s="7"/>
-      <c r="F127" s="7"/>
-      <c r="G127" s="7"/>
-      <c r="H127" s="7"/>
+      <c r="G125" s="11"/>
+      <c r="H125" s="11"/>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A126" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B126" s="11"/>
+      <c r="C126" s="4"/>
+      <c r="D126" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E126" s="3"/>
+      <c r="F126" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G126" s="11"/>
+      <c r="H126" s="11"/>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B128" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C128" s="13"/>
+      <c r="D128" s="13"/>
+      <c r="E128" s="13"/>
+      <c r="F128" s="13"/>
+      <c r="G128" s="13"/>
+      <c r="H128" s="13"/>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A129" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B128" s="7" t="s">
+      <c r="B129" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C128" s="7"/>
-      <c r="D128" s="7"/>
-      <c r="E128" s="7"/>
-      <c r="F128" s="7"/>
-      <c r="G128" s="7"/>
-      <c r="H128" s="7"/>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A129" s="8" t="s">
+      <c r="C129" s="13"/>
+      <c r="D129" s="13"/>
+      <c r="E129" s="13"/>
+      <c r="F129" s="13"/>
+      <c r="G129" s="13"/>
+      <c r="H129" s="13"/>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A130" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B129" s="8"/>
-      <c r="C129" s="8"/>
-      <c r="D129" s="8"/>
-      <c r="E129" s="8"/>
-      <c r="F129" s="8"/>
-      <c r="G129" s="8"/>
-      <c r="H129" s="8"/>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A130" s="6" t="s">
+      <c r="B130" s="14"/>
+      <c r="C130" s="14"/>
+      <c r="D130" s="14"/>
+      <c r="E130" s="14"/>
+      <c r="F130" s="14"/>
+      <c r="G130" s="14"/>
+      <c r="H130" s="14"/>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A131" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B130" s="6"/>
-      <c r="C130" s="1" t="s">
+      <c r="B131" s="12"/>
+      <c r="C131" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D130" s="1" t="s">
+      <c r="D131" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E130" s="1" t="s">
+      <c r="E131" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F130" s="1" t="s">
+      <c r="F131" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G130" s="1" t="s">
+      <c r="G131" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H130" s="1" t="s">
+      <c r="H131" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A131" s="7" t="s">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A132" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B131" s="7"/>
-      <c r="C131" s="2" t="s">
+      <c r="B132" s="13"/>
+      <c r="C132" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D131" s="2" t="s">
+      <c r="D132" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="E131" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F131" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G131" s="2"/>
-      <c r="H131" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A132" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B132" s="7"/>
-      <c r="C132" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D132" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="E132" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F132" s="2"/>
+      <c r="F132" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="G132" s="2"/>
       <c r="H132" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A133" s="7"/>
-      <c r="B133" s="7"/>
-      <c r="C133" s="2"/>
-      <c r="D133" s="2"/>
-      <c r="E133" s="2"/>
+      <c r="A133" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B133" s="13"/>
+      <c r="C133" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D133" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E133" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="F133" s="2"/>
       <c r="G133" s="2"/>
-      <c r="H133" s="2"/>
+      <c r="H133" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A134" s="7"/>
-      <c r="B134" s="7"/>
+      <c r="A134" s="13"/>
+      <c r="B134" s="13"/>
       <c r="C134" s="2"/>
       <c r="D134" s="2"/>
       <c r="E134" s="2"/>
@@ -2833,8 +2967,8 @@
       <c r="H134" s="2"/>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A135" s="7"/>
-      <c r="B135" s="7"/>
+      <c r="A135" s="13"/>
+      <c r="B135" s="13"/>
       <c r="C135" s="2"/>
       <c r="D135" s="2"/>
       <c r="E135" s="2"/>
@@ -2843,8 +2977,8 @@
       <c r="H135" s="2"/>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A136" s="7"/>
-      <c r="B136" s="7"/>
+      <c r="A136" s="13"/>
+      <c r="B136" s="13"/>
       <c r="C136" s="2"/>
       <c r="D136" s="2"/>
       <c r="E136" s="2"/>
@@ -2853,253 +2987,122 @@
       <c r="H136" s="2"/>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A137" s="6" t="s">
+      <c r="A137" s="13"/>
+      <c r="B137" s="13"/>
+      <c r="C137" s="2"/>
+      <c r="D137" s="2"/>
+      <c r="E137" s="2"/>
+      <c r="F137" s="2"/>
+      <c r="G137" s="2"/>
+      <c r="H137" s="2"/>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A138" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B137" s="6"/>
-      <c r="C137" s="6"/>
-      <c r="D137" s="6"/>
-      <c r="E137" s="6"/>
-      <c r="F137" s="6"/>
-      <c r="G137" s="6"/>
-      <c r="H137" s="6"/>
-    </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A138" s="6" t="s">
+      <c r="B138" s="12"/>
+      <c r="C138" s="12"/>
+      <c r="D138" s="12"/>
+      <c r="E138" s="12"/>
+      <c r="F138" s="12"/>
+      <c r="G138" s="12"/>
+      <c r="H138" s="12"/>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A139" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B138" s="6"/>
-      <c r="C138" s="1" t="s">
+      <c r="B139" s="12"/>
+      <c r="C139" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D138" s="1" t="s">
+      <c r="D139" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E138" s="1" t="s">
+      <c r="E139" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F138" s="6" t="s">
+      <c r="F139" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="G138" s="6"/>
-      <c r="H138" s="6"/>
-    </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A139" s="5" t="s">
+      <c r="G139" s="12"/>
+      <c r="H139" s="12"/>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A140" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B139" s="5"/>
-      <c r="C139" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D139" s="3"/>
-      <c r="E139" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F139" s="5" t="s">
+      <c r="B140" s="11"/>
+      <c r="C140" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D140" s="3"/>
+      <c r="E140" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F140" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="G139" s="5"/>
-      <c r="H139" s="5"/>
-    </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A140" s="5" t="s">
+      <c r="G140" s="11"/>
+      <c r="H140" s="11"/>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A141" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B140" s="5"/>
-      <c r="C140" s="4"/>
-      <c r="D140" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E140" s="3"/>
-      <c r="F140" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G140" s="5"/>
-      <c r="H140" s="5"/>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A141" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B141" s="5"/>
+      <c r="B141" s="11"/>
       <c r="C141" s="4"/>
       <c r="D141" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E141" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F141" s="5" t="s">
+      <c r="E141" s="3"/>
+      <c r="F141" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="G141" s="5"/>
-      <c r="H141" s="5"/>
+      <c r="G141" s="11"/>
+      <c r="H141" s="11"/>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A142" s="5" t="s">
+      <c r="A142" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B142" s="5"/>
+      <c r="B142" s="11"/>
       <c r="C142" s="4"/>
       <c r="D142" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E142" s="3"/>
-      <c r="F142" s="5" t="s">
+      <c r="E142" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F142" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="G142" s="5"/>
-      <c r="H142" s="5"/>
+      <c r="G142" s="11"/>
+      <c r="H142" s="11"/>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A143" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B143" s="11"/>
+      <c r="C143" s="4"/>
+      <c r="D143" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E143" s="3"/>
+      <c r="F143" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G143" s="11"/>
+      <c r="H143" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="174">
-    <mergeCell ref="A140:B140"/>
-    <mergeCell ref="F140:H140"/>
-    <mergeCell ref="A141:B141"/>
-    <mergeCell ref="F141:H141"/>
-    <mergeCell ref="A142:B142"/>
-    <mergeCell ref="F142:H142"/>
-    <mergeCell ref="A137:H137"/>
-    <mergeCell ref="A138:B138"/>
-    <mergeCell ref="F138:H138"/>
-    <mergeCell ref="A139:B139"/>
-    <mergeCell ref="F139:H139"/>
-    <mergeCell ref="A132:B132"/>
-    <mergeCell ref="A133:B133"/>
-    <mergeCell ref="A134:B134"/>
-    <mergeCell ref="A135:B135"/>
-    <mergeCell ref="A136:B136"/>
-    <mergeCell ref="B127:H127"/>
-    <mergeCell ref="B128:H128"/>
-    <mergeCell ref="A129:H129"/>
-    <mergeCell ref="A130:B130"/>
-    <mergeCell ref="A131:B131"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="F123:H123"/>
-    <mergeCell ref="A124:B124"/>
-    <mergeCell ref="F124:H124"/>
-    <mergeCell ref="A125:B125"/>
-    <mergeCell ref="F125:H125"/>
-    <mergeCell ref="A120:H120"/>
-    <mergeCell ref="A121:B121"/>
-    <mergeCell ref="F121:H121"/>
-    <mergeCell ref="A122:B122"/>
-    <mergeCell ref="F122:H122"/>
-    <mergeCell ref="A115:B115"/>
-    <mergeCell ref="A116:B116"/>
-    <mergeCell ref="A117:B117"/>
-    <mergeCell ref="A118:B118"/>
-    <mergeCell ref="A119:B119"/>
-    <mergeCell ref="B110:H110"/>
-    <mergeCell ref="B111:H111"/>
-    <mergeCell ref="A112:H112"/>
-    <mergeCell ref="A113:B113"/>
-    <mergeCell ref="A114:B114"/>
-    <mergeCell ref="A106:B106"/>
-    <mergeCell ref="F106:H106"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="F107:H107"/>
-    <mergeCell ref="A108:B108"/>
-    <mergeCell ref="F108:H108"/>
-    <mergeCell ref="A103:H103"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="F104:H104"/>
-    <mergeCell ref="A105:B105"/>
-    <mergeCell ref="F105:H105"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="B93:H93"/>
-    <mergeCell ref="B94:H94"/>
-    <mergeCell ref="A95:H95"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="F89:H89"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="F90:H90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="F91:H91"/>
-    <mergeCell ref="A86:H86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="F87:H87"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="F88:H88"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="B76:H76"/>
-    <mergeCell ref="B77:H77"/>
-    <mergeCell ref="A78:H78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="F72:H72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="F73:H73"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="F74:H74"/>
-    <mergeCell ref="A69:H69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="F70:H70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="F71:H71"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="B59:H59"/>
-    <mergeCell ref="B60:H60"/>
-    <mergeCell ref="A61:H61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="F55:H55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="F56:H56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="F57:H57"/>
-    <mergeCell ref="A52:H52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="F53:H53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="F54:H54"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="B43:H43"/>
-    <mergeCell ref="B44:H44"/>
-    <mergeCell ref="A45:H45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="F39:H39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="F40:H40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="F41:H41"/>
-    <mergeCell ref="A36:H36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
+  <mergeCells count="175">
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="A86:B86"/>
     <mergeCell ref="B21:H21"/>
     <mergeCell ref="B22:H22"/>
     <mergeCell ref="A23:H23"/>
@@ -3124,11 +3127,154 @@
     <mergeCell ref="F18:H18"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="F15:H15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="F39:H39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="F40:H40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="F41:H41"/>
+    <mergeCell ref="A36:H36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="B43:H43"/>
+    <mergeCell ref="B44:H44"/>
+    <mergeCell ref="A45:H45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="F55:H55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="F56:H56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="F57:H57"/>
+    <mergeCell ref="A52:H52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="F53:H53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="F54:H54"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="B59:H59"/>
+    <mergeCell ref="B60:H60"/>
+    <mergeCell ref="A61:H61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="F72:H72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="F73:H73"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="F74:H74"/>
+    <mergeCell ref="A69:H69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="F70:H70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="F71:H71"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="B76:H76"/>
+    <mergeCell ref="B77:H77"/>
+    <mergeCell ref="A78:H78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="F90:H90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="F91:H91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="F92:H92"/>
+    <mergeCell ref="A87:H87"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="F88:H88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="F89:H89"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="B94:H94"/>
+    <mergeCell ref="B95:H95"/>
+    <mergeCell ref="A96:H96"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="F107:H107"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="F108:H108"/>
+    <mergeCell ref="A109:B109"/>
+    <mergeCell ref="F109:H109"/>
+    <mergeCell ref="A104:H104"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="F105:H105"/>
+    <mergeCell ref="A106:B106"/>
+    <mergeCell ref="F106:H106"/>
+    <mergeCell ref="A116:B116"/>
+    <mergeCell ref="A117:B117"/>
+    <mergeCell ref="A118:B118"/>
+    <mergeCell ref="A119:B119"/>
+    <mergeCell ref="A120:B120"/>
+    <mergeCell ref="B111:H111"/>
+    <mergeCell ref="B112:H112"/>
+    <mergeCell ref="A113:H113"/>
+    <mergeCell ref="A114:B114"/>
+    <mergeCell ref="A115:B115"/>
+    <mergeCell ref="A124:B124"/>
+    <mergeCell ref="F124:H124"/>
+    <mergeCell ref="A125:B125"/>
+    <mergeCell ref="F125:H125"/>
+    <mergeCell ref="A126:B126"/>
+    <mergeCell ref="F126:H126"/>
+    <mergeCell ref="A121:H121"/>
+    <mergeCell ref="A122:B122"/>
+    <mergeCell ref="F122:H122"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="F123:H123"/>
+    <mergeCell ref="A133:B133"/>
+    <mergeCell ref="A134:B134"/>
+    <mergeCell ref="A135:B135"/>
+    <mergeCell ref="A136:B136"/>
+    <mergeCell ref="A137:B137"/>
+    <mergeCell ref="B128:H128"/>
+    <mergeCell ref="B129:H129"/>
+    <mergeCell ref="A130:H130"/>
+    <mergeCell ref="A131:B131"/>
+    <mergeCell ref="A132:B132"/>
+    <mergeCell ref="A141:B141"/>
+    <mergeCell ref="F141:H141"/>
+    <mergeCell ref="A142:B142"/>
+    <mergeCell ref="F142:H142"/>
+    <mergeCell ref="A143:B143"/>
+    <mergeCell ref="F143:H143"/>
+    <mergeCell ref="A138:H138"/>
+    <mergeCell ref="A139:B139"/>
+    <mergeCell ref="F139:H139"/>
+    <mergeCell ref="A140:B140"/>
+    <mergeCell ref="F140:H140"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>